<commit_message>
Documentation change for previous commit
</commit_message>
<xml_diff>
--- a/doc/core/DRV_BUS_and_more.xlsx
+++ b/doc/core/DRV_BUS_and_more.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="180" windowWidth="12900" windowHeight="8160"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="12900" windowHeight="8160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DRV_bus" sheetId="1" r:id="rId1"/>
@@ -6220,24 +6220,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6247,8 +6231,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6280,7 +6262,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6295,15 +6298,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6315,36 +6314,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6372,23 +6359,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -6692,7 +6692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
+    <sheetView topLeftCell="F49" workbookViewId="0">
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
@@ -10857,8 +10857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11011,12 +11011,12 @@
     </row>
     <row r="8" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19"/>
-      <c r="E8" s="95" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="97"/>
+      <c r="E8" s="106" t="s">
+        <v>672</v>
+      </c>
+      <c r="F8" s="107"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="108"/>
       <c r="M8" t="s">
         <v>920</v>
       </c>
@@ -11030,12 +11030,12 @@
     </row>
     <row r="9" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20"/>
-      <c r="E9" s="106" t="s">
-        <v>672</v>
-      </c>
-      <c r="F9" s="107"/>
-      <c r="G9" s="107"/>
-      <c r="H9" s="108"/>
+      <c r="E9" s="109" t="s">
+        <v>671</v>
+      </c>
+      <c r="F9" s="110"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="111"/>
       <c r="W9" s="29">
         <v>10</v>
       </c>
@@ -11048,12 +11048,12 @@
       <c r="B10" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="109" t="s">
-        <v>671</v>
-      </c>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="111"/>
+      <c r="E10" s="95" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="97"/>
       <c r="N10" s="86" t="s">
         <v>101</v>
       </c>
@@ -11199,14 +11199,14 @@
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E10:H10"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="E5:H5"/>
     <mergeCell ref="N10:P10"/>
     <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="E8:H8"/>
     <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
     <mergeCell ref="J5:P5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11218,8 +11218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:R27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24:J24"/>
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11229,11 +11229,11 @@
   <sheetData>
     <row r="6" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="121" t="s">
+      <c r="C7" s="117" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="122"/>
-      <c r="E7" s="123"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="119"/>
       <c r="J7" s="112" t="s">
         <v>83</v>
       </c>
@@ -11314,163 +11314,154 @@
       </c>
     </row>
     <row r="10" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="121" t="s">
+      <c r="C10" s="117" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="122"/>
-      <c r="E10" s="123"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="119"/>
     </row>
     <row r="11" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="126" t="s">
+      <c r="C11" s="120" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="127"/>
-      <c r="E11" s="128"/>
-      <c r="J11" s="135" t="s">
+      <c r="D11" s="121"/>
+      <c r="E11" s="122"/>
+      <c r="J11" s="129" t="s">
         <v>124</v>
       </c>
-      <c r="K11" s="136"/>
-      <c r="L11" s="137"/>
+      <c r="K11" s="130"/>
+      <c r="L11" s="131"/>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="129"/>
-      <c r="D12" s="130"/>
-      <c r="E12" s="131"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="125"/>
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12" s="138" t="s">
+      <c r="K12" s="132" t="s">
         <v>125</v>
       </c>
-      <c r="L12" s="138"/>
+      <c r="L12" s="132"/>
       <c r="M12" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="13" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="132"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="134"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="127"/>
+      <c r="E13" s="128"/>
       <c r="J13">
         <v>1</v>
       </c>
-      <c r="K13" s="138" t="s">
+      <c r="K13" s="132" t="s">
         <v>126</v>
       </c>
-      <c r="L13" s="138"/>
+      <c r="L13" s="132"/>
       <c r="M13" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125"/>
-      <c r="H20" s="124" t="s">
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="116"/>
+      <c r="H20" s="115" t="s">
         <v>147</v>
       </c>
-      <c r="I20" s="124"/>
-      <c r="J20" s="124"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="115"/>
     </row>
     <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="121"/>
-      <c r="D21" s="122"/>
-      <c r="E21" s="123"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="119"/>
       <c r="G21" t="s">
         <v>137</v>
       </c>
-      <c r="H21" s="121" t="s">
+      <c r="H21" s="117" t="s">
         <v>83</v>
       </c>
-      <c r="I21" s="122"/>
-      <c r="J21" s="123"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="119"/>
     </row>
     <row r="22" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="121"/>
-      <c r="D22" s="122"/>
-      <c r="E22" s="123"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="119"/>
       <c r="G22" t="s">
         <v>138</v>
       </c>
-      <c r="H22" s="121" t="s">
-        <v>128</v>
-      </c>
-      <c r="I22" s="122"/>
-      <c r="J22" s="123"/>
+      <c r="H22" s="117" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="118"/>
+      <c r="J22" s="119"/>
     </row>
     <row r="23" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="121"/>
-      <c r="D23" s="122"/>
-      <c r="E23" s="123"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="119"/>
       <c r="G23" t="s">
         <v>139</v>
       </c>
-      <c r="H23" s="121" t="s">
-        <v>129</v>
-      </c>
-      <c r="I23" s="122"/>
-      <c r="J23" s="123"/>
+      <c r="H23" s="117" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" s="118"/>
+      <c r="J23" s="119"/>
     </row>
     <row r="24" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="121"/>
-      <c r="D24" s="122"/>
-      <c r="E24" s="123"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="119"/>
       <c r="G24" t="s">
         <v>140</v>
       </c>
-      <c r="H24" s="121" t="s">
-        <v>101</v>
-      </c>
-      <c r="I24" s="122"/>
-      <c r="J24" s="123"/>
+      <c r="H24" s="117" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="118"/>
+      <c r="J24" s="119"/>
     </row>
     <row r="25" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="121"/>
-      <c r="D25" s="122"/>
-      <c r="E25" s="123"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="119"/>
       <c r="G25" t="s">
         <v>141</v>
       </c>
-      <c r="H25" s="121" t="s">
+      <c r="H25" s="117" t="s">
         <v>130</v>
       </c>
-      <c r="I25" s="122"/>
-      <c r="J25" s="123"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="119"/>
     </row>
     <row r="26" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="115"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="117"/>
-      <c r="H26" s="121" t="s">
+      <c r="C26" s="133"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="135"/>
+      <c r="H26" s="117" t="s">
         <v>81</v>
       </c>
-      <c r="I26" s="122"/>
-      <c r="J26" s="123"/>
+      <c r="I26" s="118"/>
+      <c r="J26" s="119"/>
     </row>
     <row r="27" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="118"/>
-      <c r="D27" s="119"/>
-      <c r="E27" s="120"/>
+      <c r="C27" s="136"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="138"/>
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27" s="121" t="s">
+      <c r="H27" s="117" t="s">
         <v>131</v>
       </c>
-      <c r="I27" s="122"/>
-      <c r="J27" s="123"/>
+      <c r="I27" s="118"/>
+      <c r="J27" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E13"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
     <mergeCell ref="C26:E27"/>
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="H26:J26"/>
@@ -11481,9 +11472,18 @@
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E13"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -11652,12 +11652,12 @@
       <c r="B2" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="140" t="s">
+      <c r="C2" s="141" t="s">
         <v>388</v>
       </c>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="143"/>
       <c r="G2" s="46" t="s">
         <v>631</v>
       </c>
@@ -11690,12 +11690,12 @@
       <c r="B4" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="144" t="s">
         <v>657</v>
       </c>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
       <c r="G4" s="43" t="s">
         <v>657</v>
       </c>
@@ -12124,12 +12124,12 @@
       <c r="B32" t="s">
         <v>641</v>
       </c>
-      <c r="C32" s="144" t="s">
+      <c r="C32" s="140" t="s">
         <v>588</v>
       </c>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
+      <c r="D32" s="140"/>
+      <c r="E32" s="140"/>
+      <c r="F32" s="140"/>
       <c r="G32" t="s">
         <v>639</v>
       </c>
@@ -12138,12 +12138,12 @@
       <c r="B33" t="s">
         <v>659</v>
       </c>
-      <c r="C33" s="144" t="s">
+      <c r="C33" s="140" t="s">
         <v>589</v>
       </c>
-      <c r="D33" s="144"/>
-      <c r="E33" s="144"/>
-      <c r="F33" s="144"/>
+      <c r="D33" s="140"/>
+      <c r="E33" s="140"/>
+      <c r="F33" s="140"/>
       <c r="G33" t="s">
         <v>640</v>
       </c>
@@ -12152,45 +12152,45 @@
       <c r="B34" t="s">
         <v>760</v>
       </c>
-      <c r="C34" s="144" t="s">
+      <c r="C34" s="140" t="s">
         <v>132</v>
       </c>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
+      <c r="D34" s="140"/>
+      <c r="E34" s="140"/>
+      <c r="F34" s="140"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>761</v>
       </c>
-      <c r="C35" s="144" t="s">
+      <c r="C35" s="140" t="s">
         <v>762</v>
       </c>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
+      <c r="D35" s="140"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="140"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>764</v>
       </c>
-      <c r="C36" s="144" t="s">
+      <c r="C36" s="140" t="s">
         <v>132</v>
       </c>
-      <c r="D36" s="144"/>
-      <c r="E36" s="144"/>
-      <c r="F36" s="144"/>
+      <c r="D36" s="140"/>
+      <c r="E36" s="140"/>
+      <c r="F36" s="140"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>765</v>
       </c>
-      <c r="C37" s="144" t="s">
+      <c r="C37" s="140" t="s">
         <v>763</v>
       </c>
-      <c r="D37" s="144"/>
-      <c r="E37" s="144"/>
-      <c r="F37" s="144"/>
+      <c r="D37" s="140"/>
+      <c r="E37" s="140"/>
+      <c r="F37" s="140"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -12283,6 +12283,35 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:E25"/>
     <mergeCell ref="C42:F42"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="C28:F28"/>
@@ -12298,35 +12327,6 @@
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -12384,16 +12384,16 @@
       <c r="L4" s="50"/>
       <c r="M4" s="50"/>
       <c r="N4" s="50"/>
-      <c r="O4" s="149" t="s">
+      <c r="O4" s="148" t="s">
         <v>388</v>
       </c>
-      <c r="P4" s="150"/>
-      <c r="Q4" s="150"/>
-      <c r="R4" s="150"/>
-      <c r="S4" s="150"/>
-      <c r="T4" s="150"/>
-      <c r="U4" s="150"/>
-      <c r="V4" s="151"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
+      <c r="R4" s="149"/>
+      <c r="S4" s="149"/>
+      <c r="T4" s="149"/>
+      <c r="U4" s="149"/>
+      <c r="V4" s="150"/>
       <c r="W4" s="147" t="s">
         <v>383</v>
       </c>
@@ -12724,14 +12724,14 @@
       <c r="D12" s="55"/>
       <c r="E12" s="55"/>
       <c r="F12" s="55"/>
-      <c r="G12" s="148" t="s">
+      <c r="G12" s="146" t="s">
         <v>558</v>
       </c>
       <c r="H12" s="139"/>
       <c r="I12" s="139"/>
       <c r="J12" s="139"/>
       <c r="K12" s="139"/>
-      <c r="L12" s="148" t="s">
+      <c r="L12" s="146" t="s">
         <v>557</v>
       </c>
       <c r="M12" s="139"/>
@@ -12942,7 +12942,7 @@
       <c r="L19" s="55"/>
       <c r="M19" s="55"/>
       <c r="N19" s="55"/>
-      <c r="O19" s="148" t="s">
+      <c r="O19" s="146" t="s">
         <v>448</v>
       </c>
       <c r="P19" s="139"/>
@@ -13004,7 +13004,7 @@
       <c r="L21" s="55"/>
       <c r="M21" s="55"/>
       <c r="N21" s="55"/>
-      <c r="O21" s="148" t="s">
+      <c r="O21" s="146" t="s">
         <v>449</v>
       </c>
       <c r="P21" s="139"/>
@@ -13033,16 +13033,16 @@
       <c r="L22" s="55"/>
       <c r="M22" s="55"/>
       <c r="N22" s="55"/>
-      <c r="O22" s="144" t="s">
+      <c r="O22" s="140" t="s">
         <v>450</v>
       </c>
-      <c r="P22" s="144"/>
-      <c r="Q22" s="144"/>
-      <c r="R22" s="144"/>
-      <c r="S22" s="144"/>
-      <c r="T22" s="144"/>
-      <c r="U22" s="144"/>
-      <c r="V22" s="144"/>
+      <c r="P22" s="140"/>
+      <c r="Q22" s="140"/>
+      <c r="R22" s="140"/>
+      <c r="S22" s="140"/>
+      <c r="T22" s="140"/>
+      <c r="U22" s="140"/>
+      <c r="V22" s="140"/>
       <c r="W22" t="s">
         <v>617</v>
       </c>
@@ -13061,7 +13061,7 @@
       <c r="K23" s="55"/>
       <c r="L23" s="55"/>
       <c r="M23" s="55"/>
-      <c r="N23" s="144" t="s">
+      <c r="N23" s="140" t="s">
         <v>457</v>
       </c>
       <c r="O23" s="145"/>
@@ -13090,7 +13090,7 @@
       <c r="K24" s="55"/>
       <c r="L24" s="55"/>
       <c r="M24" s="55"/>
-      <c r="N24" s="144" t="s">
+      <c r="N24" s="140" t="s">
         <v>458</v>
       </c>
       <c r="O24" s="145"/>
@@ -13119,7 +13119,7 @@
       <c r="K25" s="55"/>
       <c r="L25" s="55"/>
       <c r="M25" s="55"/>
-      <c r="N25" s="144" t="s">
+      <c r="N25" s="140" t="s">
         <v>459</v>
       </c>
       <c r="O25" s="145"/>
@@ -13148,7 +13148,7 @@
       <c r="K26" s="55"/>
       <c r="L26" s="55"/>
       <c r="M26" s="55"/>
-      <c r="N26" s="144" t="s">
+      <c r="N26" s="140" t="s">
         <v>460</v>
       </c>
       <c r="O26" s="145"/>
@@ -13185,17 +13185,17 @@
       <c r="M27" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="N27" s="144" t="s">
+      <c r="N27" s="140" t="s">
         <v>464</v>
       </c>
-      <c r="O27" s="144"/>
-      <c r="P27" s="144"/>
-      <c r="Q27" s="144"/>
-      <c r="R27" s="144"/>
-      <c r="S27" s="144"/>
-      <c r="T27" s="144"/>
-      <c r="U27" s="144"/>
-      <c r="V27" s="144"/>
+      <c r="O27" s="140"/>
+      <c r="P27" s="140"/>
+      <c r="Q27" s="140"/>
+      <c r="R27" s="140"/>
+      <c r="S27" s="140"/>
+      <c r="T27" s="140"/>
+      <c r="U27" s="140"/>
+      <c r="V27" s="140"/>
       <c r="W27">
         <v>0</v>
       </c>
@@ -13646,17 +13646,17 @@
       <c r="C43" t="s">
         <v>531</v>
       </c>
-      <c r="D43" s="146"/>
-      <c r="E43" s="146"/>
-      <c r="F43" s="146"/>
-      <c r="G43" s="146"/>
-      <c r="H43" s="146"/>
-      <c r="I43" s="146"/>
-      <c r="J43" s="146"/>
-      <c r="K43" s="146"/>
-      <c r="L43" s="146"/>
-      <c r="M43" s="146"/>
-      <c r="N43" s="146"/>
+      <c r="D43" s="151"/>
+      <c r="E43" s="151"/>
+      <c r="F43" s="151"/>
+      <c r="G43" s="151"/>
+      <c r="H43" s="151"/>
+      <c r="I43" s="151"/>
+      <c r="J43" s="151"/>
+      <c r="K43" s="151"/>
+      <c r="L43" s="151"/>
+      <c r="M43" s="151"/>
+      <c r="N43" s="151"/>
       <c r="O43" s="139" t="s">
         <v>532</v>
       </c>
@@ -13679,17 +13679,17 @@
       <c r="C44" t="s">
         <v>544</v>
       </c>
-      <c r="D44" s="146"/>
-      <c r="E44" s="146"/>
-      <c r="F44" s="146"/>
-      <c r="G44" s="146"/>
-      <c r="H44" s="146"/>
-      <c r="I44" s="146"/>
-      <c r="J44" s="146"/>
-      <c r="K44" s="146"/>
-      <c r="L44" s="146"/>
-      <c r="M44" s="146"/>
-      <c r="N44" s="146"/>
+      <c r="D44" s="151"/>
+      <c r="E44" s="151"/>
+      <c r="F44" s="151"/>
+      <c r="G44" s="151"/>
+      <c r="H44" s="151"/>
+      <c r="I44" s="151"/>
+      <c r="J44" s="151"/>
+      <c r="K44" s="151"/>
+      <c r="L44" s="151"/>
+      <c r="M44" s="151"/>
+      <c r="N44" s="151"/>
       <c r="O44" s="139" t="s">
         <v>132</v>
       </c>
@@ -13915,6 +13915,47 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="D45:V45"/>
+    <mergeCell ref="D46:V46"/>
+    <mergeCell ref="D43:N43"/>
+    <mergeCell ref="D44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="O43:T43"/>
+    <mergeCell ref="G42:V42"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="O21:V21"/>
+    <mergeCell ref="O19:V19"/>
+    <mergeCell ref="O22:V22"/>
+    <mergeCell ref="O4:V4"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="R16:V16"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="Q12:V12"/>
+    <mergeCell ref="L12:P12"/>
+    <mergeCell ref="O18:V18"/>
+    <mergeCell ref="Q14:V14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:V15"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="O39:V39"/>
+    <mergeCell ref="O40:V40"/>
+    <mergeCell ref="D41:V41"/>
+    <mergeCell ref="E30:V30"/>
+    <mergeCell ref="E31:V31"/>
+    <mergeCell ref="E32:V32"/>
+    <mergeCell ref="N26:V26"/>
+    <mergeCell ref="N25:V25"/>
+    <mergeCell ref="E29:V29"/>
+    <mergeCell ref="O35:T35"/>
+    <mergeCell ref="O36:V36"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="S13:V13"/>
+    <mergeCell ref="Q13:R13"/>
     <mergeCell ref="D51:V51"/>
     <mergeCell ref="G20:S20"/>
     <mergeCell ref="O37:V37"/>
@@ -13931,47 +13972,6 @@
     <mergeCell ref="G47:N47"/>
     <mergeCell ref="O48:V48"/>
     <mergeCell ref="O34:R34"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="O39:V39"/>
-    <mergeCell ref="O40:V40"/>
-    <mergeCell ref="D41:V41"/>
-    <mergeCell ref="E30:V30"/>
-    <mergeCell ref="E31:V31"/>
-    <mergeCell ref="E32:V32"/>
-    <mergeCell ref="N26:V26"/>
-    <mergeCell ref="N25:V25"/>
-    <mergeCell ref="E29:V29"/>
-    <mergeCell ref="O35:T35"/>
-    <mergeCell ref="O36:V36"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="S13:V13"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="O21:V21"/>
-    <mergeCell ref="O19:V19"/>
-    <mergeCell ref="O22:V22"/>
-    <mergeCell ref="O4:V4"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="R16:V16"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="Q12:V12"/>
-    <mergeCell ref="L12:P12"/>
-    <mergeCell ref="O18:V18"/>
-    <mergeCell ref="Q14:V14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:V15"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="D45:V45"/>
-    <mergeCell ref="D46:V46"/>
-    <mergeCell ref="D43:N43"/>
-    <mergeCell ref="D44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="O43:T43"/>
-    <mergeCell ref="G42:V42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -13994,33 +13994,33 @@
   <sheetData>
     <row r="2" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C3" s="158" t="s">
+      <c r="C3" s="170" t="s">
         <v>812</v>
       </c>
-      <c r="D3" s="159"/>
+      <c r="D3" s="171"/>
       <c r="E3" s="63"/>
       <c r="F3" s="63"/>
       <c r="G3" s="63"/>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
-      <c r="J3" s="153" t="s">
+      <c r="J3" s="172" t="s">
         <v>388</v>
       </c>
-      <c r="K3" s="153"/>
-      <c r="L3" s="153"/>
-      <c r="M3" s="153"/>
-      <c r="N3" s="153"/>
-      <c r="O3" s="153"/>
-      <c r="P3" s="153"/>
-      <c r="Q3" s="153"/>
-      <c r="R3" s="153"/>
-      <c r="S3" s="153"/>
-      <c r="T3" s="153"/>
-      <c r="U3" s="153"/>
-      <c r="V3" s="153"/>
-      <c r="W3" s="153"/>
-      <c r="X3" s="153"/>
-      <c r="Y3" s="160"/>
+      <c r="K3" s="172"/>
+      <c r="L3" s="172"/>
+      <c r="M3" s="172"/>
+      <c r="N3" s="172"/>
+      <c r="O3" s="172"/>
+      <c r="P3" s="172"/>
+      <c r="Q3" s="172"/>
+      <c r="R3" s="172"/>
+      <c r="S3" s="172"/>
+      <c r="T3" s="172"/>
+      <c r="U3" s="172"/>
+      <c r="V3" s="172"/>
+      <c r="W3" s="172"/>
+      <c r="X3" s="172"/>
+      <c r="Y3" s="173"/>
     </row>
     <row r="4" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C4" s="64"/>
@@ -14090,10 +14090,10 @@
       </c>
     </row>
     <row r="5" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C5" s="156" t="s">
+      <c r="C5" s="168" t="s">
         <v>810</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="169"/>
       <c r="E5" s="66"/>
       <c r="F5" s="66"/>
       <c r="G5" s="66"/>
@@ -14153,10 +14153,10 @@
       </c>
     </row>
     <row r="6" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="156" t="s">
+      <c r="C6" s="168" t="s">
         <v>811</v>
       </c>
-      <c r="D6" s="157"/>
+      <c r="D6" s="169"/>
       <c r="E6" s="66" t="s">
         <v>835</v>
       </c>
@@ -14222,35 +14222,35 @@
       </c>
     </row>
     <row r="7" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="118" t="s">
+      <c r="C7" s="136" t="s">
         <v>900</v>
       </c>
-      <c r="D7" s="119"/>
+      <c r="D7" s="137"/>
       <c r="E7" s="67"/>
       <c r="F7" s="67"/>
       <c r="G7" s="67"/>
       <c r="H7" s="67"/>
       <c r="I7" s="67"/>
-      <c r="J7" s="161" t="s">
+      <c r="J7" s="174" t="s">
         <v>873</v>
       </c>
-      <c r="K7" s="162"/>
-      <c r="L7" s="162"/>
-      <c r="M7" s="162"/>
-      <c r="N7" s="162"/>
-      <c r="O7" s="162"/>
-      <c r="P7" s="162"/>
-      <c r="Q7" s="163"/>
-      <c r="R7" s="177" t="s">
+      <c r="K7" s="175"/>
+      <c r="L7" s="175"/>
+      <c r="M7" s="175"/>
+      <c r="N7" s="175"/>
+      <c r="O7" s="175"/>
+      <c r="P7" s="175"/>
+      <c r="Q7" s="176"/>
+      <c r="R7" s="156" t="s">
         <v>836</v>
       </c>
-      <c r="S7" s="178"/>
-      <c r="T7" s="178"/>
-      <c r="U7" s="178"/>
-      <c r="V7" s="178"/>
-      <c r="W7" s="178"/>
-      <c r="X7" s="178"/>
-      <c r="Y7" s="179"/>
+      <c r="S7" s="157"/>
+      <c r="T7" s="157"/>
+      <c r="U7" s="157"/>
+      <c r="V7" s="157"/>
+      <c r="W7" s="157"/>
+      <c r="X7" s="157"/>
+      <c r="Y7" s="158"/>
     </row>
     <row r="11" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="139" t="s">
@@ -14269,27 +14269,27 @@
         <v>791</v>
       </c>
       <c r="F12" s="139"/>
-      <c r="N12" s="170" t="s">
+      <c r="N12" s="165" t="s">
         <v>836</v>
       </c>
-      <c r="O12" s="171"/>
-      <c r="P12" s="171"/>
-      <c r="Q12" s="172"/>
+      <c r="O12" s="166"/>
+      <c r="P12" s="166"/>
+      <c r="Q12" s="167"/>
       <c r="R12" s="71" t="s">
         <v>837</v>
       </c>
-      <c r="S12" s="154" t="s">
+      <c r="S12" s="177" t="s">
         <v>866</v>
       </c>
-      <c r="T12" s="155"/>
+      <c r="T12" s="178"/>
     </row>
     <row r="13" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="N13" s="167" t="s">
+      <c r="N13" s="162" t="s">
         <v>813</v>
       </c>
-      <c r="O13" s="168"/>
-      <c r="P13" s="168"/>
-      <c r="Q13" s="169"/>
+      <c r="O13" s="163"/>
+      <c r="P13" s="163"/>
+      <c r="Q13" s="164"/>
       <c r="R13" t="s">
         <v>838</v>
       </c>
@@ -14299,12 +14299,12 @@
       <c r="T13" s="145"/>
     </row>
     <row r="14" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="N14" s="164" t="s">
+      <c r="N14" s="159" t="s">
         <v>435</v>
       </c>
-      <c r="O14" s="165"/>
-      <c r="P14" s="165"/>
-      <c r="Q14" s="166"/>
+      <c r="O14" s="160"/>
+      <c r="P14" s="160"/>
+      <c r="Q14" s="161"/>
       <c r="R14" t="s">
         <v>839</v>
       </c>
@@ -14314,12 +14314,12 @@
       <c r="T14" s="145"/>
     </row>
     <row r="15" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="N15" s="164" t="s">
+      <c r="N15" s="159" t="s">
         <v>854</v>
       </c>
-      <c r="O15" s="165"/>
-      <c r="P15" s="165"/>
-      <c r="Q15" s="166"/>
+      <c r="O15" s="160"/>
+      <c r="P15" s="160"/>
+      <c r="Q15" s="161"/>
       <c r="R15" t="s">
         <v>840</v>
       </c>
@@ -14329,12 +14329,12 @@
       <c r="T15" s="145"/>
     </row>
     <row r="16" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N16" s="164" t="s">
+      <c r="N16" s="159" t="s">
         <v>855</v>
       </c>
-      <c r="O16" s="165"/>
-      <c r="P16" s="165"/>
-      <c r="Q16" s="166"/>
+      <c r="O16" s="160"/>
+      <c r="P16" s="160"/>
+      <c r="Q16" s="161"/>
       <c r="R16" t="s">
         <v>411</v>
       </c>
@@ -14368,12 +14368,12 @@
       <c r="K17" s="52">
         <v>0</v>
       </c>
-      <c r="N17" s="164" t="s">
+      <c r="N17" s="159" t="s">
         <v>817</v>
       </c>
-      <c r="O17" s="165"/>
-      <c r="P17" s="165"/>
-      <c r="Q17" s="166"/>
+      <c r="O17" s="160"/>
+      <c r="P17" s="160"/>
+      <c r="Q17" s="161"/>
       <c r="R17" t="s">
         <v>841</v>
       </c>
@@ -14386,11 +14386,11 @@
       <c r="C18" t="s">
         <v>868</v>
       </c>
-      <c r="D18" s="153" t="s">
+      <c r="D18" s="172" t="s">
         <v>132</v>
       </c>
-      <c r="E18" s="153"/>
-      <c r="F18" s="153"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
       <c r="G18" t="s">
         <v>878</v>
       </c>
@@ -14406,19 +14406,19 @@
       <c r="K18" t="s">
         <v>874</v>
       </c>
-      <c r="N18" s="164" t="s">
+      <c r="N18" s="159" t="s">
         <v>816</v>
       </c>
-      <c r="O18" s="165"/>
-      <c r="P18" s="165"/>
-      <c r="Q18" s="166"/>
+      <c r="O18" s="160"/>
+      <c r="P18" s="160"/>
+      <c r="Q18" s="161"/>
       <c r="R18" t="s">
         <v>842</v>
       </c>
-      <c r="S18" s="152" t="s">
+      <c r="S18" s="179" t="s">
         <v>868</v>
       </c>
-      <c r="T18" s="152"/>
+      <c r="T18" s="179"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
@@ -14438,19 +14438,19 @@
       <c r="K19" t="s">
         <v>880</v>
       </c>
-      <c r="N19" s="164" t="s">
+      <c r="N19" s="159" t="s">
         <v>818</v>
       </c>
-      <c r="O19" s="165"/>
-      <c r="P19" s="165"/>
-      <c r="Q19" s="166"/>
+      <c r="O19" s="160"/>
+      <c r="P19" s="160"/>
+      <c r="Q19" s="161"/>
       <c r="R19" t="s">
         <v>843</v>
       </c>
-      <c r="S19" s="152" t="s">
+      <c r="S19" s="179" t="s">
         <v>869</v>
       </c>
-      <c r="T19" s="152"/>
+      <c r="T19" s="179"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
@@ -14474,12 +14474,12 @@
       <c r="K20" t="s">
         <v>881</v>
       </c>
-      <c r="N20" s="164" t="s">
+      <c r="N20" s="159" t="s">
         <v>820</v>
       </c>
-      <c r="O20" s="165"/>
-      <c r="P20" s="165"/>
-      <c r="Q20" s="166"/>
+      <c r="O20" s="160"/>
+      <c r="P20" s="160"/>
+      <c r="Q20" s="161"/>
       <c r="R20" t="s">
         <v>438</v>
       </c>
@@ -14506,12 +14506,12 @@
       </c>
       <c r="J21" s="139"/>
       <c r="K21" s="139"/>
-      <c r="N21" s="164" t="s">
+      <c r="N21" s="159" t="s">
         <v>821</v>
       </c>
-      <c r="O21" s="165"/>
-      <c r="P21" s="165"/>
-      <c r="Q21" s="166"/>
+      <c r="O21" s="160"/>
+      <c r="P21" s="160"/>
+      <c r="Q21" s="161"/>
       <c r="R21" t="s">
         <v>844</v>
       </c>
@@ -14538,12 +14538,12 @@
       </c>
       <c r="J22" s="139"/>
       <c r="K22" s="139"/>
-      <c r="N22" s="164" t="s">
+      <c r="N22" s="159" t="s">
         <v>822</v>
       </c>
-      <c r="O22" s="165"/>
-      <c r="P22" s="165"/>
-      <c r="Q22" s="166"/>
+      <c r="O22" s="160"/>
+      <c r="P22" s="160"/>
+      <c r="Q22" s="161"/>
       <c r="R22" t="s">
         <v>846</v>
       </c>
@@ -14553,27 +14553,27 @@
       <c r="T22" s="145"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N23" s="164" t="s">
+      <c r="N23" s="159" t="s">
         <v>823</v>
       </c>
-      <c r="O23" s="165"/>
-      <c r="P23" s="165"/>
-      <c r="Q23" s="166"/>
+      <c r="O23" s="160"/>
+      <c r="P23" s="160"/>
+      <c r="Q23" s="161"/>
       <c r="R23" t="s">
         <v>847</v>
       </c>
-      <c r="S23" s="152" t="s">
+      <c r="S23" s="179" t="s">
         <v>618</v>
       </c>
-      <c r="T23" s="152"/>
+      <c r="T23" s="179"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N24" s="164" t="s">
+      <c r="N24" s="159" t="s">
         <v>824</v>
       </c>
-      <c r="O24" s="165"/>
-      <c r="P24" s="165"/>
-      <c r="Q24" s="166"/>
+      <c r="O24" s="160"/>
+      <c r="P24" s="160"/>
+      <c r="Q24" s="161"/>
       <c r="R24" t="s">
         <v>439</v>
       </c>
@@ -14583,12 +14583,12 @@
       <c r="T24" s="145"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N25" s="164" t="s">
+      <c r="N25" s="159" t="s">
         <v>825</v>
       </c>
-      <c r="O25" s="165"/>
-      <c r="P25" s="165"/>
-      <c r="Q25" s="166"/>
+      <c r="O25" s="160"/>
+      <c r="P25" s="160"/>
+      <c r="Q25" s="161"/>
       <c r="R25" t="s">
         <v>848</v>
       </c>
@@ -14598,12 +14598,12 @@
       <c r="T25" s="145"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N26" s="164" t="s">
+      <c r="N26" s="159" t="s">
         <v>826</v>
       </c>
-      <c r="O26" s="165"/>
-      <c r="P26" s="165"/>
-      <c r="Q26" s="166"/>
+      <c r="O26" s="160"/>
+      <c r="P26" s="160"/>
+      <c r="Q26" s="161"/>
       <c r="R26" t="s">
         <v>849</v>
       </c>
@@ -14613,12 +14613,12 @@
       <c r="T26" s="145"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N27" s="164" t="s">
+      <c r="N27" s="159" t="s">
         <v>827</v>
       </c>
-      <c r="O27" s="165"/>
-      <c r="P27" s="165"/>
-      <c r="Q27" s="166"/>
+      <c r="O27" s="160"/>
+      <c r="P27" s="160"/>
+      <c r="Q27" s="161"/>
       <c r="R27" t="s">
         <v>850</v>
       </c>
@@ -14628,12 +14628,12 @@
       <c r="T27" s="145"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N28" s="164" t="s">
+      <c r="N28" s="159" t="s">
         <v>830</v>
       </c>
-      <c r="O28" s="165"/>
-      <c r="P28" s="165"/>
-      <c r="Q28" s="166"/>
+      <c r="O28" s="160"/>
+      <c r="P28" s="160"/>
+      <c r="Q28" s="161"/>
       <c r="R28" t="s">
         <v>441</v>
       </c>
@@ -14643,12 +14643,12 @@
       <c r="T28" s="145"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N29" s="164" t="s">
+      <c r="N29" s="159" t="s">
         <v>831</v>
       </c>
-      <c r="O29" s="165"/>
-      <c r="P29" s="165"/>
-      <c r="Q29" s="166"/>
+      <c r="O29" s="160"/>
+      <c r="P29" s="160"/>
+      <c r="Q29" s="161"/>
       <c r="R29" t="s">
         <v>845</v>
       </c>
@@ -14658,57 +14658,57 @@
       <c r="T29" s="145"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N30" s="164" t="s">
+      <c r="N30" s="159" t="s">
         <v>832</v>
       </c>
-      <c r="O30" s="165"/>
-      <c r="P30" s="165"/>
-      <c r="Q30" s="166"/>
+      <c r="O30" s="160"/>
+      <c r="P30" s="160"/>
+      <c r="Q30" s="161"/>
       <c r="R30" t="s">
         <v>851</v>
       </c>
-      <c r="S30" s="152" t="s">
+      <c r="S30" s="179" t="s">
         <v>870</v>
       </c>
-      <c r="T30" s="152"/>
+      <c r="T30" s="179"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N31" s="164" t="s">
+      <c r="N31" s="159" t="s">
         <v>833</v>
       </c>
-      <c r="O31" s="165"/>
-      <c r="P31" s="165"/>
-      <c r="Q31" s="166"/>
+      <c r="O31" s="160"/>
+      <c r="P31" s="160"/>
+      <c r="Q31" s="161"/>
       <c r="R31" t="s">
         <v>852</v>
       </c>
-      <c r="S31" s="152" t="s">
+      <c r="S31" s="179" t="s">
         <v>871</v>
       </c>
-      <c r="T31" s="152"/>
+      <c r="T31" s="179"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N32" s="164" t="s">
+      <c r="N32" s="159" t="s">
         <v>856</v>
       </c>
-      <c r="O32" s="165"/>
-      <c r="P32" s="165"/>
-      <c r="Q32" s="166"/>
+      <c r="O32" s="160"/>
+      <c r="P32" s="160"/>
+      <c r="Q32" s="161"/>
       <c r="R32" t="s">
         <v>451</v>
       </c>
-      <c r="S32" s="152" t="s">
+      <c r="S32" s="179" t="s">
         <v>872</v>
       </c>
-      <c r="T32" s="152"/>
+      <c r="T32" s="179"/>
     </row>
     <row r="33" spans="14:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N33" s="173" t="s">
+      <c r="N33" s="152" t="s">
         <v>835</v>
       </c>
-      <c r="O33" s="174"/>
-      <c r="P33" s="174"/>
-      <c r="Q33" s="175"/>
+      <c r="O33" s="153"/>
+      <c r="P33" s="153"/>
+      <c r="Q33" s="154"/>
       <c r="R33" t="s">
         <v>853</v>
       </c>
@@ -14716,19 +14716,67 @@
         <v>618</v>
       </c>
       <c r="T33" s="145"/>
-      <c r="U33" s="176"/>
-      <c r="V33" s="176"/>
-      <c r="W33" s="176"/>
-      <c r="X33" s="176"/>
+      <c r="U33" s="155"/>
+      <c r="V33" s="155"/>
+      <c r="W33" s="155"/>
+      <c r="X33" s="155"/>
     </row>
     <row r="34" spans="14:24" x14ac:dyDescent="0.25">
-      <c r="U34" s="176"/>
-      <c r="V34" s="176"/>
-      <c r="W34" s="176"/>
-      <c r="X34" s="176"/>
+      <c r="U34" s="155"/>
+      <c r="V34" s="155"/>
+      <c r="W34" s="155"/>
+      <c r="X34" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J3:Y3"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
     <mergeCell ref="N33:Q33"/>
     <mergeCell ref="U33:X33"/>
     <mergeCell ref="U34:X34"/>
@@ -14745,54 +14793,6 @@
     <mergeCell ref="N24:Q24"/>
     <mergeCell ref="N25:Q25"/>
     <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J3:Y3"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="J7:Q7"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="S22:T22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Documentation update for previous commit
</commit_message>
<xml_diff>
--- a/doc/core/DRV_BUS_and_more.xlsx
+++ b/doc/core/DRV_BUS_and_more.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="180" windowWidth="12900" windowHeight="8160" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="12900" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DRV_bus" sheetId="1" r:id="rId1"/>
@@ -2515,7 +2515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="938">
   <si>
     <t>Index</t>
   </si>
@@ -5253,9 +5253,6 @@
     <t>FD_TYPE</t>
   </si>
   <si>
-    <t>107-90</t>
-  </si>
-  <si>
     <t>272-257</t>
   </si>
   <si>
@@ -5320,6 +5317,18 @@
   </si>
   <si>
     <t>Logic 1 indicates that data from Avalon access will be written into TX Buffer 2</t>
+  </si>
+  <si>
+    <t>99-90</t>
+  </si>
+  <si>
+    <t>107-100</t>
+  </si>
+  <si>
+    <t>err_capt</t>
+  </si>
+  <si>
+    <t>Error capture register</t>
   </si>
 </sst>
 </file>
@@ -6220,8 +6229,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6231,6 +6256,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6262,28 +6289,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6298,11 +6304,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6314,24 +6324,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6359,36 +6381,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -7451,7 +7460,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D34" s="9">
         <v>0</v>
@@ -7463,7 +7472,7 @@
         <v>134</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H34" s="9"/>
     </row>
@@ -7498,7 +7507,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D36" s="9">
         <v>0</v>
@@ -7510,7 +7519,7 @@
         <v>134</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="H36" s="9"/>
     </row>
@@ -9551,10 +9560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10178,10 +10187,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="39" t="s">
-        <v>912</v>
+        <v>934</v>
       </c>
       <c r="B35" s="43">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C35" s="43" t="s">
         <v>168</v>
@@ -10190,640 +10199,641 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="39" t="s">
+        <v>935</v>
+      </c>
+      <c r="B36" s="43">
+        <v>8</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>936</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>937</v>
+      </c>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
         <v>600</v>
       </c>
-      <c r="B36" s="43">
+      <c r="B37" s="43">
         <v>2</v>
       </c>
-      <c r="C36" s="43" t="s">
+      <c r="C37" s="43" t="s">
         <v>336</v>
       </c>
-      <c r="D36" s="9">
-        <v>0</v>
-      </c>
-      <c r="E36" s="43" t="s">
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="43" t="s">
         <v>337</v>
       </c>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="39">
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="39">
         <v>110</v>
-      </c>
-      <c r="B37" s="43">
-        <v>1</v>
-      </c>
-      <c r="C37" s="43" t="s">
-        <v>338</v>
-      </c>
-      <c r="D37" s="9">
-        <v>0</v>
-      </c>
-      <c r="E37" s="43" t="s">
-        <v>339</v>
-      </c>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
-        <v>111</v>
       </c>
       <c r="B38" s="43">
         <v>1</v>
       </c>
       <c r="C38" s="43" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D38" s="9">
         <v>0</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B39" s="43">
         <v>1</v>
       </c>
       <c r="C39" s="43" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D39" s="9">
         <v>0</v>
       </c>
       <c r="E39" s="43" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B40" s="43">
         <v>1</v>
       </c>
       <c r="C40" s="43" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D40" s="9">
         <v>0</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" s="43">
         <v>1</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D41" s="9">
         <v>0</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B42" s="43">
         <v>1</v>
       </c>
       <c r="C42" s="43" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D42" s="9">
         <v>0</v>
       </c>
       <c r="E42" s="43" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43" s="43">
         <v>1</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D43" s="9">
         <v>0</v>
       </c>
       <c r="E43" s="43" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B44" s="43">
         <v>1</v>
       </c>
       <c r="C44" s="43" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D44" s="9">
         <v>0</v>
       </c>
       <c r="E44" s="43" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B45" s="43">
         <v>1</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D45" s="9">
         <v>0</v>
       </c>
       <c r="E45" s="43" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B46" s="43">
         <v>1</v>
       </c>
       <c r="C46" s="43" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D46" s="9">
         <v>0</v>
       </c>
       <c r="E46" s="43" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B47" s="43">
         <v>1</v>
       </c>
       <c r="C47" s="43" t="s">
+        <v>356</v>
+      </c>
+      <c r="D47" s="9">
+        <v>0</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>357</v>
+      </c>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
+        <v>120</v>
+      </c>
+      <c r="B48" s="43">
+        <v>1</v>
+      </c>
+      <c r="C48" s="43" t="s">
         <v>358</v>
       </c>
-      <c r="D47" s="9">
-        <v>0</v>
-      </c>
-      <c r="E47" s="43" t="s">
+      <c r="D48" s="9">
+        <v>0</v>
+      </c>
+      <c r="E48" s="43" t="s">
         <v>359</v>
-      </c>
-      <c r="F47" s="9"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>601</v>
-      </c>
-      <c r="B48" s="43">
-        <v>29</v>
-      </c>
-      <c r="C48" s="43" t="s">
-        <v>367</v>
-      </c>
-      <c r="D48" s="9">
-        <v>0</v>
-      </c>
-      <c r="E48" s="43" t="s">
-        <v>360</v>
       </c>
       <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="B49" s="43">
+        <v>29</v>
+      </c>
+      <c r="C49" s="43" t="s">
+        <v>367</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0</v>
+      </c>
+      <c r="E49" s="43" t="s">
+        <v>360</v>
+      </c>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>602</v>
       </c>
-      <c r="B49" s="43">
+      <c r="B50" s="43">
         <v>4</v>
       </c>
-      <c r="C49" s="43" t="s">
+      <c r="C50" s="43" t="s">
         <v>368</v>
       </c>
-      <c r="D49" s="9">
-        <v>0</v>
-      </c>
-      <c r="E49" s="43" t="s">
+      <c r="D50" s="9">
+        <v>0</v>
+      </c>
+      <c r="E50" s="43" t="s">
         <v>361</v>
-      </c>
-      <c r="F49" s="9"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
-        <v>154</v>
-      </c>
-      <c r="B50" s="43">
-        <v>1</v>
-      </c>
-      <c r="C50" s="43" t="s">
-        <v>369</v>
-      </c>
-      <c r="D50" s="9">
-        <v>0</v>
-      </c>
-      <c r="E50" s="43" t="s">
-        <v>362</v>
       </c>
       <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B51" s="43">
         <v>1</v>
       </c>
       <c r="C51" s="43" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D51" s="9">
         <v>0</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B52" s="43">
         <v>1</v>
       </c>
       <c r="C52" s="43" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="D52" s="9">
         <v>0</v>
       </c>
       <c r="E52" s="43" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B53" s="43">
         <v>1</v>
       </c>
       <c r="C53" s="43" t="s">
+        <v>367</v>
+      </c>
+      <c r="D53" s="9">
+        <v>0</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>364</v>
+      </c>
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>157</v>
+      </c>
+      <c r="B54" s="43">
+        <v>1</v>
+      </c>
+      <c r="C54" s="43" t="s">
         <v>371</v>
       </c>
-      <c r="D53" s="9">
-        <v>0</v>
-      </c>
-      <c r="E53" s="43" t="s">
+      <c r="D54" s="9">
+        <v>0</v>
+      </c>
+      <c r="E54" s="43" t="s">
         <v>365</v>
       </c>
-      <c r="F53" s="9"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>603</v>
       </c>
-      <c r="B54" s="43">
+      <c r="B55" s="43">
         <v>21</v>
       </c>
-      <c r="C54" s="43" t="s">
+      <c r="C55" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="D54" s="9">
-        <v>0</v>
-      </c>
-      <c r="E54" s="43" t="s">
+      <c r="D55" s="9">
+        <v>0</v>
+      </c>
+      <c r="E55" s="43" t="s">
         <v>366</v>
-      </c>
-      <c r="F54" s="9"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
-        <v>179</v>
-      </c>
-      <c r="B55" s="43">
-        <v>1</v>
-      </c>
-      <c r="C55" s="43" t="s">
-        <v>377</v>
-      </c>
-      <c r="D55" s="9">
-        <v>0</v>
-      </c>
-      <c r="E55" s="43" t="s">
-        <v>378</v>
       </c>
       <c r="F55" s="9"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B56" s="43">
         <v>1</v>
       </c>
       <c r="C56" s="43" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D56" s="9">
         <v>0</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B57" s="43">
         <v>1</v>
       </c>
       <c r="C57" s="43" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="D57" s="9">
         <v>0</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B58" s="43">
         <v>1</v>
       </c>
       <c r="C58" s="43" t="s">
+        <v>373</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0</v>
+      </c>
+      <c r="E58" s="43" t="s">
+        <v>374</v>
+      </c>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>182</v>
+      </c>
+      <c r="B59" s="43">
+        <v>1</v>
+      </c>
+      <c r="C59" s="43" t="s">
         <v>375</v>
       </c>
-      <c r="D58" s="9">
-        <v>0</v>
-      </c>
-      <c r="E58" s="43" t="s">
+      <c r="D59" s="9">
+        <v>0</v>
+      </c>
+      <c r="E59" s="43" t="s">
         <v>376</v>
-      </c>
-      <c r="F58" s="9"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
-        <v>604</v>
-      </c>
-      <c r="B59" s="43">
-        <v>5</v>
-      </c>
-      <c r="C59" s="43" t="s">
-        <v>575</v>
-      </c>
-      <c r="D59" s="9">
-        <v>0</v>
-      </c>
-      <c r="E59" s="43" t="s">
-        <v>576</v>
       </c>
       <c r="F59" s="9"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B60" s="43">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="D60" s="9">
         <v>0</v>
       </c>
       <c r="E60" s="43" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="F60" s="9"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B61" s="43">
         <v>32</v>
       </c>
       <c r="C61" s="43" t="s">
+        <v>583</v>
+      </c>
+      <c r="D61" s="9">
+        <v>0</v>
+      </c>
+      <c r="E61" s="43" t="s">
+        <v>584</v>
+      </c>
+      <c r="F61" s="9"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="B62" s="43">
+        <v>32</v>
+      </c>
+      <c r="C62" s="43" t="s">
         <v>585</v>
       </c>
-      <c r="D61" s="9">
-        <v>0</v>
-      </c>
-      <c r="E61" s="43" t="s">
+      <c r="D62" s="9">
+        <v>0</v>
+      </c>
+      <c r="E62" s="43" t="s">
         <v>586</v>
-      </c>
-      <c r="F61" s="9"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
-        <v>252</v>
-      </c>
-      <c r="B62" s="43">
-        <v>1</v>
-      </c>
-      <c r="C62" s="43" t="s">
-        <v>802</v>
-      </c>
-      <c r="D62" s="9">
-        <v>0</v>
-      </c>
-      <c r="E62" s="43" t="s">
-        <v>803</v>
       </c>
       <c r="F62" s="9"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B63" s="43">
         <v>1</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D63" s="9">
         <v>0</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F63" s="9"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B64" s="43">
         <v>1</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D64" s="9">
         <v>0</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F64" s="9"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B65" s="43">
         <v>1</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>890</v>
+        <v>806</v>
       </c>
       <c r="D65" s="9">
         <v>0</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>891</v>
+        <v>807</v>
       </c>
       <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B66" s="43">
         <v>1</v>
       </c>
       <c r="C66" s="43" t="s">
+        <v>890</v>
+      </c>
+      <c r="D66" s="9">
+        <v>0</v>
+      </c>
+      <c r="E66" s="43" t="s">
+        <v>891</v>
+      </c>
+      <c r="F66" s="9"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
+        <v>256</v>
+      </c>
+      <c r="B67" s="43">
+        <v>1</v>
+      </c>
+      <c r="C67" s="43" t="s">
         <v>892</v>
       </c>
-      <c r="D66" s="9"/>
-      <c r="E66" s="43" t="s">
+      <c r="D67" s="9"/>
+      <c r="E67" s="43" t="s">
         <v>889</v>
-      </c>
-      <c r="F66" s="9"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="39" t="s">
-        <v>913</v>
-      </c>
-      <c r="B67" s="43">
-        <v>16</v>
-      </c>
-      <c r="C67" s="43" t="s">
-        <v>653</v>
-      </c>
-      <c r="D67" s="9">
-        <v>0</v>
-      </c>
-      <c r="E67" s="43" t="s">
-        <v>656</v>
       </c>
       <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="39" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B68" s="43">
         <v>16</v>
       </c>
       <c r="C68" s="43" t="s">
+        <v>653</v>
+      </c>
+      <c r="D68" s="9">
+        <v>0</v>
+      </c>
+      <c r="E68" s="43" t="s">
+        <v>656</v>
+      </c>
+      <c r="F68" s="9"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="39" t="s">
+        <v>913</v>
+      </c>
+      <c r="B69" s="43">
+        <v>16</v>
+      </c>
+      <c r="C69" s="43" t="s">
         <v>654</v>
       </c>
-      <c r="D68" s="9">
-        <v>0</v>
-      </c>
-      <c r="E68" s="43" t="s">
+      <c r="D69" s="9">
+        <v>0</v>
+      </c>
+      <c r="E69" s="43" t="s">
         <v>655</v>
       </c>
-      <c r="F68" s="9"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>921</v>
-      </c>
-      <c r="B69" s="43">
-        <v>11</v>
-      </c>
-      <c r="C69" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="D69" s="9">
-        <v>0</v>
-      </c>
-      <c r="E69" s="9"/>
       <c r="F69" s="9"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="B70" s="43">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C70" s="43" t="s">
-        <v>923</v>
+        <v>168</v>
       </c>
       <c r="D70" s="9">
         <v>0</v>
       </c>
-      <c r="E70" s="9" t="s">
-        <v>927</v>
-      </c>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="B71" s="43">
         <v>3</v>
       </c>
       <c r="C71" s="43" t="s">
-        <v>925</v>
-      </c>
-      <c r="D71">
+        <v>922</v>
+      </c>
+      <c r="D71" s="9">
         <v>0</v>
       </c>
       <c r="E71" s="9" t="s">
@@ -10832,16 +10842,33 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
+        <v>923</v>
+      </c>
+      <c r="B72" s="43">
+        <v>3</v>
+      </c>
+      <c r="C72" s="43" t="s">
+        <v>924</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>927</v>
+      </c>
+      <c r="B73" s="43">
+        <v>64</v>
+      </c>
+      <c r="C73" s="43" t="s">
         <v>928</v>
       </c>
-      <c r="B72" s="43">
-        <v>64</v>
-      </c>
-      <c r="C72" s="43" t="s">
+      <c r="E73" s="9" t="s">
         <v>929</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>930</v>
       </c>
     </row>
   </sheetData>
@@ -10857,7 +10884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -10916,16 +10943,16 @@
       <c r="G6" s="99"/>
       <c r="H6" s="100"/>
       <c r="J6" t="s">
+        <v>914</v>
+      </c>
+      <c r="K6" s="77" t="s">
+        <v>918</v>
+      </c>
+      <c r="L6" s="77" t="s">
+        <v>917</v>
+      </c>
+      <c r="M6" s="77" t="s">
         <v>915</v>
-      </c>
-      <c r="K6" s="77" t="s">
-        <v>919</v>
-      </c>
-      <c r="L6" s="77" t="s">
-        <v>918</v>
-      </c>
-      <c r="M6" s="77" t="s">
-        <v>916</v>
       </c>
       <c r="N6" s="24" t="s">
         <v>117</v>
@@ -10969,7 +10996,7 @@
         <v>114</v>
       </c>
       <c r="K7" s="77" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="L7" s="77" t="s">
         <v>818</v>
@@ -11018,7 +11045,7 @@
       <c r="G8" s="107"/>
       <c r="H8" s="108"/>
       <c r="M8" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="W8" s="29">
         <v>1</v>
@@ -11229,11 +11256,11 @@
   <sheetData>
     <row r="6" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="117" t="s">
+      <c r="C7" s="121" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="118"/>
-      <c r="E7" s="119"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="123"/>
       <c r="J7" s="112" t="s">
         <v>83</v>
       </c>
@@ -11314,154 +11341,163 @@
       </c>
     </row>
     <row r="10" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="117" t="s">
+      <c r="C10" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="118"/>
-      <c r="E10" s="119"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="123"/>
     </row>
     <row r="11" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="126" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="121"/>
-      <c r="E11" s="122"/>
-      <c r="J11" s="129" t="s">
+      <c r="D11" s="127"/>
+      <c r="E11" s="128"/>
+      <c r="J11" s="135" t="s">
         <v>124</v>
       </c>
-      <c r="K11" s="130"/>
-      <c r="L11" s="131"/>
+      <c r="K11" s="136"/>
+      <c r="L11" s="137"/>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="123"/>
-      <c r="D12" s="124"/>
-      <c r="E12" s="125"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="131"/>
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12" s="132" t="s">
+      <c r="K12" s="138" t="s">
         <v>125</v>
       </c>
-      <c r="L12" s="132"/>
+      <c r="L12" s="138"/>
       <c r="M12" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="13" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="126"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="128"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="133"/>
+      <c r="E13" s="134"/>
       <c r="J13">
         <v>1</v>
       </c>
-      <c r="K13" s="132" t="s">
+      <c r="K13" s="138" t="s">
         <v>126</v>
       </c>
-      <c r="L13" s="132"/>
+      <c r="L13" s="138"/>
       <c r="M13" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="116"/>
-      <c r="H20" s="115" t="s">
+      <c r="C20" s="125"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="H20" s="124" t="s">
         <v>147</v>
       </c>
-      <c r="I20" s="115"/>
-      <c r="J20" s="115"/>
+      <c r="I20" s="124"/>
+      <c r="J20" s="124"/>
     </row>
     <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="117"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="119"/>
+      <c r="C21" s="121"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="123"/>
       <c r="G21" t="s">
         <v>137</v>
       </c>
-      <c r="H21" s="117" t="s">
+      <c r="H21" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="I21" s="118"/>
-      <c r="J21" s="119"/>
+      <c r="I21" s="122"/>
+      <c r="J21" s="123"/>
     </row>
     <row r="22" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="117"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="119"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="122"/>
+      <c r="E22" s="123"/>
       <c r="G22" t="s">
         <v>138</v>
       </c>
-      <c r="H22" s="117" t="s">
+      <c r="H22" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="I22" s="118"/>
-      <c r="J22" s="119"/>
+      <c r="I22" s="122"/>
+      <c r="J22" s="123"/>
     </row>
     <row r="23" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="117"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="119"/>
+      <c r="C23" s="121"/>
+      <c r="D23" s="122"/>
+      <c r="E23" s="123"/>
       <c r="G23" t="s">
         <v>139</v>
       </c>
-      <c r="H23" s="117" t="s">
+      <c r="H23" s="121" t="s">
         <v>128</v>
       </c>
-      <c r="I23" s="118"/>
-      <c r="J23" s="119"/>
+      <c r="I23" s="122"/>
+      <c r="J23" s="123"/>
     </row>
     <row r="24" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="117"/>
-      <c r="D24" s="118"/>
-      <c r="E24" s="119"/>
+      <c r="C24" s="121"/>
+      <c r="D24" s="122"/>
+      <c r="E24" s="123"/>
       <c r="G24" t="s">
         <v>140</v>
       </c>
-      <c r="H24" s="117" t="s">
+      <c r="H24" s="121" t="s">
         <v>129</v>
       </c>
-      <c r="I24" s="118"/>
-      <c r="J24" s="119"/>
+      <c r="I24" s="122"/>
+      <c r="J24" s="123"/>
     </row>
     <row r="25" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="117"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="119"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="123"/>
       <c r="G25" t="s">
         <v>141</v>
       </c>
-      <c r="H25" s="117" t="s">
+      <c r="H25" s="121" t="s">
         <v>130</v>
       </c>
-      <c r="I25" s="118"/>
-      <c r="J25" s="119"/>
+      <c r="I25" s="122"/>
+      <c r="J25" s="123"/>
     </row>
     <row r="26" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="133"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="135"/>
-      <c r="H26" s="117" t="s">
+      <c r="C26" s="115"/>
+      <c r="D26" s="116"/>
+      <c r="E26" s="117"/>
+      <c r="H26" s="121" t="s">
         <v>81</v>
       </c>
-      <c r="I26" s="118"/>
-      <c r="J26" s="119"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="123"/>
     </row>
     <row r="27" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="136"/>
-      <c r="D27" s="137"/>
-      <c r="E27" s="138"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="120"/>
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27" s="117" t="s">
+      <c r="H27" s="121" t="s">
         <v>131</v>
       </c>
-      <c r="I27" s="118"/>
-      <c r="J27" s="119"/>
+      <c r="I27" s="122"/>
+      <c r="J27" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E13"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
     <mergeCell ref="C26:E27"/>
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="H26:J26"/>
@@ -11475,15 +11511,6 @@
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E13"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -11652,12 +11679,12 @@
       <c r="B2" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="141" t="s">
+      <c r="C2" s="140" t="s">
         <v>388</v>
       </c>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="143"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="142"/>
       <c r="G2" s="46" t="s">
         <v>631</v>
       </c>
@@ -11690,12 +11717,12 @@
       <c r="B4" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="143" t="s">
         <v>657</v>
       </c>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
       <c r="G4" s="43" t="s">
         <v>657</v>
       </c>
@@ -12124,12 +12151,12 @@
       <c r="B32" t="s">
         <v>641</v>
       </c>
-      <c r="C32" s="140" t="s">
+      <c r="C32" s="144" t="s">
         <v>588</v>
       </c>
-      <c r="D32" s="140"/>
-      <c r="E32" s="140"/>
-      <c r="F32" s="140"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="144"/>
       <c r="G32" t="s">
         <v>639</v>
       </c>
@@ -12138,12 +12165,12 @@
       <c r="B33" t="s">
         <v>659</v>
       </c>
-      <c r="C33" s="140" t="s">
+      <c r="C33" s="144" t="s">
         <v>589</v>
       </c>
-      <c r="D33" s="140"/>
-      <c r="E33" s="140"/>
-      <c r="F33" s="140"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="144"/>
+      <c r="F33" s="144"/>
       <c r="G33" t="s">
         <v>640</v>
       </c>
@@ -12152,45 +12179,45 @@
       <c r="B34" t="s">
         <v>760</v>
       </c>
-      <c r="C34" s="140" t="s">
+      <c r="C34" s="144" t="s">
         <v>132</v>
       </c>
-      <c r="D34" s="140"/>
-      <c r="E34" s="140"/>
-      <c r="F34" s="140"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="144"/>
+      <c r="F34" s="144"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>761</v>
       </c>
-      <c r="C35" s="140" t="s">
+      <c r="C35" s="144" t="s">
         <v>762</v>
       </c>
-      <c r="D35" s="140"/>
-      <c r="E35" s="140"/>
-      <c r="F35" s="140"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="144"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>764</v>
       </c>
-      <c r="C36" s="140" t="s">
+      <c r="C36" s="144" t="s">
         <v>132</v>
       </c>
-      <c r="D36" s="140"/>
-      <c r="E36" s="140"/>
-      <c r="F36" s="140"/>
+      <c r="D36" s="144"/>
+      <c r="E36" s="144"/>
+      <c r="F36" s="144"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>765</v>
       </c>
-      <c r="C37" s="140" t="s">
+      <c r="C37" s="144" t="s">
         <v>763</v>
       </c>
-      <c r="D37" s="140"/>
-      <c r="E37" s="140"/>
-      <c r="F37" s="140"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="144"/>
+      <c r="F37" s="144"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -12283,35 +12310,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C25:E25"/>
     <mergeCell ref="C42:F42"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="C28:F28"/>
@@ -12327,6 +12325,35 @@
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -12384,16 +12411,16 @@
       <c r="L4" s="50"/>
       <c r="M4" s="50"/>
       <c r="N4" s="50"/>
-      <c r="O4" s="148" t="s">
+      <c r="O4" s="149" t="s">
         <v>388</v>
       </c>
-      <c r="P4" s="149"/>
-      <c r="Q4" s="149"/>
-      <c r="R4" s="149"/>
-      <c r="S4" s="149"/>
-      <c r="T4" s="149"/>
-      <c r="U4" s="149"/>
-      <c r="V4" s="150"/>
+      <c r="P4" s="150"/>
+      <c r="Q4" s="150"/>
+      <c r="R4" s="150"/>
+      <c r="S4" s="150"/>
+      <c r="T4" s="150"/>
+      <c r="U4" s="150"/>
+      <c r="V4" s="151"/>
       <c r="W4" s="147" t="s">
         <v>383</v>
       </c>
@@ -12724,14 +12751,14 @@
       <c r="D12" s="55"/>
       <c r="E12" s="55"/>
       <c r="F12" s="55"/>
-      <c r="G12" s="146" t="s">
+      <c r="G12" s="148" t="s">
         <v>558</v>
       </c>
       <c r="H12" s="139"/>
       <c r="I12" s="139"/>
       <c r="J12" s="139"/>
       <c r="K12" s="139"/>
-      <c r="L12" s="146" t="s">
+      <c r="L12" s="148" t="s">
         <v>557</v>
       </c>
       <c r="M12" s="139"/>
@@ -12942,7 +12969,7 @@
       <c r="L19" s="55"/>
       <c r="M19" s="55"/>
       <c r="N19" s="55"/>
-      <c r="O19" s="146" t="s">
+      <c r="O19" s="148" t="s">
         <v>448</v>
       </c>
       <c r="P19" s="139"/>
@@ -13004,7 +13031,7 @@
       <c r="L21" s="55"/>
       <c r="M21" s="55"/>
       <c r="N21" s="55"/>
-      <c r="O21" s="146" t="s">
+      <c r="O21" s="148" t="s">
         <v>449</v>
       </c>
       <c r="P21" s="139"/>
@@ -13033,16 +13060,16 @@
       <c r="L22" s="55"/>
       <c r="M22" s="55"/>
       <c r="N22" s="55"/>
-      <c r="O22" s="140" t="s">
+      <c r="O22" s="144" t="s">
         <v>450</v>
       </c>
-      <c r="P22" s="140"/>
-      <c r="Q22" s="140"/>
-      <c r="R22" s="140"/>
-      <c r="S22" s="140"/>
-      <c r="T22" s="140"/>
-      <c r="U22" s="140"/>
-      <c r="V22" s="140"/>
+      <c r="P22" s="144"/>
+      <c r="Q22" s="144"/>
+      <c r="R22" s="144"/>
+      <c r="S22" s="144"/>
+      <c r="T22" s="144"/>
+      <c r="U22" s="144"/>
+      <c r="V22" s="144"/>
       <c r="W22" t="s">
         <v>617</v>
       </c>
@@ -13061,7 +13088,7 @@
       <c r="K23" s="55"/>
       <c r="L23" s="55"/>
       <c r="M23" s="55"/>
-      <c r="N23" s="140" t="s">
+      <c r="N23" s="144" t="s">
         <v>457</v>
       </c>
       <c r="O23" s="145"/>
@@ -13090,7 +13117,7 @@
       <c r="K24" s="55"/>
       <c r="L24" s="55"/>
       <c r="M24" s="55"/>
-      <c r="N24" s="140" t="s">
+      <c r="N24" s="144" t="s">
         <v>458</v>
       </c>
       <c r="O24" s="145"/>
@@ -13119,7 +13146,7 @@
       <c r="K25" s="55"/>
       <c r="L25" s="55"/>
       <c r="M25" s="55"/>
-      <c r="N25" s="140" t="s">
+      <c r="N25" s="144" t="s">
         <v>459</v>
       </c>
       <c r="O25" s="145"/>
@@ -13148,7 +13175,7 @@
       <c r="K26" s="55"/>
       <c r="L26" s="55"/>
       <c r="M26" s="55"/>
-      <c r="N26" s="140" t="s">
+      <c r="N26" s="144" t="s">
         <v>460</v>
       </c>
       <c r="O26" s="145"/>
@@ -13185,17 +13212,17 @@
       <c r="M27" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="N27" s="140" t="s">
+      <c r="N27" s="144" t="s">
         <v>464</v>
       </c>
-      <c r="O27" s="140"/>
-      <c r="P27" s="140"/>
-      <c r="Q27" s="140"/>
-      <c r="R27" s="140"/>
-      <c r="S27" s="140"/>
-      <c r="T27" s="140"/>
-      <c r="U27" s="140"/>
-      <c r="V27" s="140"/>
+      <c r="O27" s="144"/>
+      <c r="P27" s="144"/>
+      <c r="Q27" s="144"/>
+      <c r="R27" s="144"/>
+      <c r="S27" s="144"/>
+      <c r="T27" s="144"/>
+      <c r="U27" s="144"/>
+      <c r="V27" s="144"/>
       <c r="W27">
         <v>0</v>
       </c>
@@ -13646,17 +13673,17 @@
       <c r="C43" t="s">
         <v>531</v>
       </c>
-      <c r="D43" s="151"/>
-      <c r="E43" s="151"/>
-      <c r="F43" s="151"/>
-      <c r="G43" s="151"/>
-      <c r="H43" s="151"/>
-      <c r="I43" s="151"/>
-      <c r="J43" s="151"/>
-      <c r="K43" s="151"/>
-      <c r="L43" s="151"/>
-      <c r="M43" s="151"/>
-      <c r="N43" s="151"/>
+      <c r="D43" s="146"/>
+      <c r="E43" s="146"/>
+      <c r="F43" s="146"/>
+      <c r="G43" s="146"/>
+      <c r="H43" s="146"/>
+      <c r="I43" s="146"/>
+      <c r="J43" s="146"/>
+      <c r="K43" s="146"/>
+      <c r="L43" s="146"/>
+      <c r="M43" s="146"/>
+      <c r="N43" s="146"/>
       <c r="O43" s="139" t="s">
         <v>532</v>
       </c>
@@ -13679,17 +13706,17 @@
       <c r="C44" t="s">
         <v>544</v>
       </c>
-      <c r="D44" s="151"/>
-      <c r="E44" s="151"/>
-      <c r="F44" s="151"/>
-      <c r="G44" s="151"/>
-      <c r="H44" s="151"/>
-      <c r="I44" s="151"/>
-      <c r="J44" s="151"/>
-      <c r="K44" s="151"/>
-      <c r="L44" s="151"/>
-      <c r="M44" s="151"/>
-      <c r="N44" s="151"/>
+      <c r="D44" s="146"/>
+      <c r="E44" s="146"/>
+      <c r="F44" s="146"/>
+      <c r="G44" s="146"/>
+      <c r="H44" s="146"/>
+      <c r="I44" s="146"/>
+      <c r="J44" s="146"/>
+      <c r="K44" s="146"/>
+      <c r="L44" s="146"/>
+      <c r="M44" s="146"/>
+      <c r="N44" s="146"/>
       <c r="O44" s="139" t="s">
         <v>132</v>
       </c>
@@ -13915,15 +13942,38 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="D45:V45"/>
-    <mergeCell ref="D46:V46"/>
-    <mergeCell ref="D43:N43"/>
-    <mergeCell ref="D44:N44"/>
-    <mergeCell ref="O44:R44"/>
-    <mergeCell ref="O43:T43"/>
-    <mergeCell ref="G42:V42"/>
+    <mergeCell ref="D51:V51"/>
+    <mergeCell ref="G20:S20"/>
+    <mergeCell ref="O37:V37"/>
+    <mergeCell ref="O38:V38"/>
+    <mergeCell ref="E33:V33"/>
+    <mergeCell ref="S34:V34"/>
+    <mergeCell ref="N24:V24"/>
+    <mergeCell ref="N23:V23"/>
+    <mergeCell ref="O49:V49"/>
+    <mergeCell ref="O50:R50"/>
+    <mergeCell ref="O47:S47"/>
+    <mergeCell ref="N27:V27"/>
+    <mergeCell ref="E28:V28"/>
+    <mergeCell ref="G47:N47"/>
+    <mergeCell ref="O48:V48"/>
+    <mergeCell ref="O34:R34"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="O39:V39"/>
+    <mergeCell ref="O40:V40"/>
+    <mergeCell ref="D41:V41"/>
+    <mergeCell ref="E30:V30"/>
+    <mergeCell ref="E31:V31"/>
+    <mergeCell ref="E32:V32"/>
+    <mergeCell ref="N26:V26"/>
+    <mergeCell ref="N25:V25"/>
+    <mergeCell ref="E29:V29"/>
+    <mergeCell ref="O35:T35"/>
+    <mergeCell ref="O36:V36"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="S13:V13"/>
+    <mergeCell ref="Q13:R13"/>
     <mergeCell ref="W4:X4"/>
     <mergeCell ref="O21:V21"/>
     <mergeCell ref="O19:V19"/>
@@ -13940,38 +13990,15 @@
     <mergeCell ref="O14:P14"/>
     <mergeCell ref="O15:P15"/>
     <mergeCell ref="Q15:V15"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="O39:V39"/>
-    <mergeCell ref="O40:V40"/>
-    <mergeCell ref="D41:V41"/>
-    <mergeCell ref="E30:V30"/>
-    <mergeCell ref="E31:V31"/>
-    <mergeCell ref="E32:V32"/>
-    <mergeCell ref="N26:V26"/>
-    <mergeCell ref="N25:V25"/>
-    <mergeCell ref="E29:V29"/>
-    <mergeCell ref="O35:T35"/>
-    <mergeCell ref="O36:V36"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="S13:V13"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="D51:V51"/>
-    <mergeCell ref="G20:S20"/>
-    <mergeCell ref="O37:V37"/>
-    <mergeCell ref="O38:V38"/>
-    <mergeCell ref="E33:V33"/>
-    <mergeCell ref="S34:V34"/>
-    <mergeCell ref="N24:V24"/>
-    <mergeCell ref="N23:V23"/>
-    <mergeCell ref="O49:V49"/>
-    <mergeCell ref="O50:R50"/>
-    <mergeCell ref="O47:S47"/>
-    <mergeCell ref="N27:V27"/>
-    <mergeCell ref="E28:V28"/>
-    <mergeCell ref="G47:N47"/>
-    <mergeCell ref="O48:V48"/>
-    <mergeCell ref="O34:R34"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="D45:V45"/>
+    <mergeCell ref="D46:V46"/>
+    <mergeCell ref="D43:N43"/>
+    <mergeCell ref="D44:N44"/>
+    <mergeCell ref="O44:R44"/>
+    <mergeCell ref="O43:T43"/>
+    <mergeCell ref="G42:V42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -13994,33 +14021,33 @@
   <sheetData>
     <row r="2" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C3" s="170" t="s">
+      <c r="C3" s="158" t="s">
         <v>812</v>
       </c>
-      <c r="D3" s="171"/>
+      <c r="D3" s="159"/>
       <c r="E3" s="63"/>
       <c r="F3" s="63"/>
       <c r="G3" s="63"/>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
-      <c r="J3" s="172" t="s">
+      <c r="J3" s="153" t="s">
         <v>388</v>
       </c>
-      <c r="K3" s="172"/>
-      <c r="L3" s="172"/>
-      <c r="M3" s="172"/>
-      <c r="N3" s="172"/>
-      <c r="O3" s="172"/>
-      <c r="P3" s="172"/>
-      <c r="Q3" s="172"/>
-      <c r="R3" s="172"/>
-      <c r="S3" s="172"/>
-      <c r="T3" s="172"/>
-      <c r="U3" s="172"/>
-      <c r="V3" s="172"/>
-      <c r="W3" s="172"/>
-      <c r="X3" s="172"/>
-      <c r="Y3" s="173"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
+      <c r="Q3" s="153"/>
+      <c r="R3" s="153"/>
+      <c r="S3" s="153"/>
+      <c r="T3" s="153"/>
+      <c r="U3" s="153"/>
+      <c r="V3" s="153"/>
+      <c r="W3" s="153"/>
+      <c r="X3" s="153"/>
+      <c r="Y3" s="160"/>
     </row>
     <row r="4" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C4" s="64"/>
@@ -14090,10 +14117,10 @@
       </c>
     </row>
     <row r="5" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C5" s="168" t="s">
+      <c r="C5" s="156" t="s">
         <v>810</v>
       </c>
-      <c r="D5" s="169"/>
+      <c r="D5" s="157"/>
       <c r="E5" s="66"/>
       <c r="F5" s="66"/>
       <c r="G5" s="66"/>
@@ -14153,10 +14180,10 @@
       </c>
     </row>
     <row r="6" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="168" t="s">
+      <c r="C6" s="156" t="s">
         <v>811</v>
       </c>
-      <c r="D6" s="169"/>
+      <c r="D6" s="157"/>
       <c r="E6" s="66" t="s">
         <v>835</v>
       </c>
@@ -14222,35 +14249,35 @@
       </c>
     </row>
     <row r="7" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="136" t="s">
+      <c r="C7" s="118" t="s">
         <v>900</v>
       </c>
-      <c r="D7" s="137"/>
+      <c r="D7" s="119"/>
       <c r="E7" s="67"/>
       <c r="F7" s="67"/>
       <c r="G7" s="67"/>
       <c r="H7" s="67"/>
       <c r="I7" s="67"/>
-      <c r="J7" s="174" t="s">
+      <c r="J7" s="161" t="s">
         <v>873</v>
       </c>
-      <c r="K7" s="175"/>
-      <c r="L7" s="175"/>
-      <c r="M7" s="175"/>
-      <c r="N7" s="175"/>
-      <c r="O7" s="175"/>
-      <c r="P7" s="175"/>
-      <c r="Q7" s="176"/>
-      <c r="R7" s="156" t="s">
+      <c r="K7" s="162"/>
+      <c r="L7" s="162"/>
+      <c r="M7" s="162"/>
+      <c r="N7" s="162"/>
+      <c r="O7" s="162"/>
+      <c r="P7" s="162"/>
+      <c r="Q7" s="163"/>
+      <c r="R7" s="177" t="s">
         <v>836</v>
       </c>
-      <c r="S7" s="157"/>
-      <c r="T7" s="157"/>
-      <c r="U7" s="157"/>
-      <c r="V7" s="157"/>
-      <c r="W7" s="157"/>
-      <c r="X7" s="157"/>
-      <c r="Y7" s="158"/>
+      <c r="S7" s="178"/>
+      <c r="T7" s="178"/>
+      <c r="U7" s="178"/>
+      <c r="V7" s="178"/>
+      <c r="W7" s="178"/>
+      <c r="X7" s="178"/>
+      <c r="Y7" s="179"/>
     </row>
     <row r="11" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="139" t="s">
@@ -14269,27 +14296,27 @@
         <v>791</v>
       </c>
       <c r="F12" s="139"/>
-      <c r="N12" s="165" t="s">
+      <c r="N12" s="170" t="s">
         <v>836</v>
       </c>
-      <c r="O12" s="166"/>
-      <c r="P12" s="166"/>
-      <c r="Q12" s="167"/>
+      <c r="O12" s="171"/>
+      <c r="P12" s="171"/>
+      <c r="Q12" s="172"/>
       <c r="R12" s="71" t="s">
         <v>837</v>
       </c>
-      <c r="S12" s="177" t="s">
+      <c r="S12" s="154" t="s">
         <v>866</v>
       </c>
-      <c r="T12" s="178"/>
+      <c r="T12" s="155"/>
     </row>
     <row r="13" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="N13" s="162" t="s">
+      <c r="N13" s="167" t="s">
         <v>813</v>
       </c>
-      <c r="O13" s="163"/>
-      <c r="P13" s="163"/>
-      <c r="Q13" s="164"/>
+      <c r="O13" s="168"/>
+      <c r="P13" s="168"/>
+      <c r="Q13" s="169"/>
       <c r="R13" t="s">
         <v>838</v>
       </c>
@@ -14299,12 +14326,12 @@
       <c r="T13" s="145"/>
     </row>
     <row r="14" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="N14" s="159" t="s">
+      <c r="N14" s="164" t="s">
         <v>435</v>
       </c>
-      <c r="O14" s="160"/>
-      <c r="P14" s="160"/>
-      <c r="Q14" s="161"/>
+      <c r="O14" s="165"/>
+      <c r="P14" s="165"/>
+      <c r="Q14" s="166"/>
       <c r="R14" t="s">
         <v>839</v>
       </c>
@@ -14314,12 +14341,12 @@
       <c r="T14" s="145"/>
     </row>
     <row r="15" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="N15" s="159" t="s">
+      <c r="N15" s="164" t="s">
         <v>854</v>
       </c>
-      <c r="O15" s="160"/>
-      <c r="P15" s="160"/>
-      <c r="Q15" s="161"/>
+      <c r="O15" s="165"/>
+      <c r="P15" s="165"/>
+      <c r="Q15" s="166"/>
       <c r="R15" t="s">
         <v>840</v>
       </c>
@@ -14329,12 +14356,12 @@
       <c r="T15" s="145"/>
     </row>
     <row r="16" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N16" s="159" t="s">
+      <c r="N16" s="164" t="s">
         <v>855</v>
       </c>
-      <c r="O16" s="160"/>
-      <c r="P16" s="160"/>
-      <c r="Q16" s="161"/>
+      <c r="O16" s="165"/>
+      <c r="P16" s="165"/>
+      <c r="Q16" s="166"/>
       <c r="R16" t="s">
         <v>411</v>
       </c>
@@ -14368,12 +14395,12 @@
       <c r="K17" s="52">
         <v>0</v>
       </c>
-      <c r="N17" s="159" t="s">
+      <c r="N17" s="164" t="s">
         <v>817</v>
       </c>
-      <c r="O17" s="160"/>
-      <c r="P17" s="160"/>
-      <c r="Q17" s="161"/>
+      <c r="O17" s="165"/>
+      <c r="P17" s="165"/>
+      <c r="Q17" s="166"/>
       <c r="R17" t="s">
         <v>841</v>
       </c>
@@ -14386,11 +14413,11 @@
       <c r="C18" t="s">
         <v>868</v>
       </c>
-      <c r="D18" s="172" t="s">
+      <c r="D18" s="153" t="s">
         <v>132</v>
       </c>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
+      <c r="E18" s="153"/>
+      <c r="F18" s="153"/>
       <c r="G18" t="s">
         <v>878</v>
       </c>
@@ -14406,19 +14433,19 @@
       <c r="K18" t="s">
         <v>874</v>
       </c>
-      <c r="N18" s="159" t="s">
+      <c r="N18" s="164" t="s">
         <v>816</v>
       </c>
-      <c r="O18" s="160"/>
-      <c r="P18" s="160"/>
-      <c r="Q18" s="161"/>
+      <c r="O18" s="165"/>
+      <c r="P18" s="165"/>
+      <c r="Q18" s="166"/>
       <c r="R18" t="s">
         <v>842</v>
       </c>
-      <c r="S18" s="179" t="s">
+      <c r="S18" s="152" t="s">
         <v>868</v>
       </c>
-      <c r="T18" s="179"/>
+      <c r="T18" s="152"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
@@ -14438,19 +14465,19 @@
       <c r="K19" t="s">
         <v>880</v>
       </c>
-      <c r="N19" s="159" t="s">
+      <c r="N19" s="164" t="s">
         <v>818</v>
       </c>
-      <c r="O19" s="160"/>
-      <c r="P19" s="160"/>
-      <c r="Q19" s="161"/>
+      <c r="O19" s="165"/>
+      <c r="P19" s="165"/>
+      <c r="Q19" s="166"/>
       <c r="R19" t="s">
         <v>843</v>
       </c>
-      <c r="S19" s="179" t="s">
+      <c r="S19" s="152" t="s">
         <v>869</v>
       </c>
-      <c r="T19" s="179"/>
+      <c r="T19" s="152"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
@@ -14474,12 +14501,12 @@
       <c r="K20" t="s">
         <v>881</v>
       </c>
-      <c r="N20" s="159" t="s">
+      <c r="N20" s="164" t="s">
         <v>820</v>
       </c>
-      <c r="O20" s="160"/>
-      <c r="P20" s="160"/>
-      <c r="Q20" s="161"/>
+      <c r="O20" s="165"/>
+      <c r="P20" s="165"/>
+      <c r="Q20" s="166"/>
       <c r="R20" t="s">
         <v>438</v>
       </c>
@@ -14506,12 +14533,12 @@
       </c>
       <c r="J21" s="139"/>
       <c r="K21" s="139"/>
-      <c r="N21" s="159" t="s">
+      <c r="N21" s="164" t="s">
         <v>821</v>
       </c>
-      <c r="O21" s="160"/>
-      <c r="P21" s="160"/>
-      <c r="Q21" s="161"/>
+      <c r="O21" s="165"/>
+      <c r="P21" s="165"/>
+      <c r="Q21" s="166"/>
       <c r="R21" t="s">
         <v>844</v>
       </c>
@@ -14538,12 +14565,12 @@
       </c>
       <c r="J22" s="139"/>
       <c r="K22" s="139"/>
-      <c r="N22" s="159" t="s">
+      <c r="N22" s="164" t="s">
         <v>822</v>
       </c>
-      <c r="O22" s="160"/>
-      <c r="P22" s="160"/>
-      <c r="Q22" s="161"/>
+      <c r="O22" s="165"/>
+      <c r="P22" s="165"/>
+      <c r="Q22" s="166"/>
       <c r="R22" t="s">
         <v>846</v>
       </c>
@@ -14553,27 +14580,27 @@
       <c r="T22" s="145"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N23" s="159" t="s">
+      <c r="N23" s="164" t="s">
         <v>823</v>
       </c>
-      <c r="O23" s="160"/>
-      <c r="P23" s="160"/>
-      <c r="Q23" s="161"/>
+      <c r="O23" s="165"/>
+      <c r="P23" s="165"/>
+      <c r="Q23" s="166"/>
       <c r="R23" t="s">
         <v>847</v>
       </c>
-      <c r="S23" s="179" t="s">
+      <c r="S23" s="152" t="s">
         <v>618</v>
       </c>
-      <c r="T23" s="179"/>
+      <c r="T23" s="152"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N24" s="159" t="s">
+      <c r="N24" s="164" t="s">
         <v>824</v>
       </c>
-      <c r="O24" s="160"/>
-      <c r="P24" s="160"/>
-      <c r="Q24" s="161"/>
+      <c r="O24" s="165"/>
+      <c r="P24" s="165"/>
+      <c r="Q24" s="166"/>
       <c r="R24" t="s">
         <v>439</v>
       </c>
@@ -14583,12 +14610,12 @@
       <c r="T24" s="145"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N25" s="159" t="s">
+      <c r="N25" s="164" t="s">
         <v>825</v>
       </c>
-      <c r="O25" s="160"/>
-      <c r="P25" s="160"/>
-      <c r="Q25" s="161"/>
+      <c r="O25" s="165"/>
+      <c r="P25" s="165"/>
+      <c r="Q25" s="166"/>
       <c r="R25" t="s">
         <v>848</v>
       </c>
@@ -14598,12 +14625,12 @@
       <c r="T25" s="145"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N26" s="159" t="s">
+      <c r="N26" s="164" t="s">
         <v>826</v>
       </c>
-      <c r="O26" s="160"/>
-      <c r="P26" s="160"/>
-      <c r="Q26" s="161"/>
+      <c r="O26" s="165"/>
+      <c r="P26" s="165"/>
+      <c r="Q26" s="166"/>
       <c r="R26" t="s">
         <v>849</v>
       </c>
@@ -14613,12 +14640,12 @@
       <c r="T26" s="145"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N27" s="159" t="s">
+      <c r="N27" s="164" t="s">
         <v>827</v>
       </c>
-      <c r="O27" s="160"/>
-      <c r="P27" s="160"/>
-      <c r="Q27" s="161"/>
+      <c r="O27" s="165"/>
+      <c r="P27" s="165"/>
+      <c r="Q27" s="166"/>
       <c r="R27" t="s">
         <v>850</v>
       </c>
@@ -14628,12 +14655,12 @@
       <c r="T27" s="145"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N28" s="159" t="s">
+      <c r="N28" s="164" t="s">
         <v>830</v>
       </c>
-      <c r="O28" s="160"/>
-      <c r="P28" s="160"/>
-      <c r="Q28" s="161"/>
+      <c r="O28" s="165"/>
+      <c r="P28" s="165"/>
+      <c r="Q28" s="166"/>
       <c r="R28" t="s">
         <v>441</v>
       </c>
@@ -14643,12 +14670,12 @@
       <c r="T28" s="145"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N29" s="159" t="s">
+      <c r="N29" s="164" t="s">
         <v>831</v>
       </c>
-      <c r="O29" s="160"/>
-      <c r="P29" s="160"/>
-      <c r="Q29" s="161"/>
+      <c r="O29" s="165"/>
+      <c r="P29" s="165"/>
+      <c r="Q29" s="166"/>
       <c r="R29" t="s">
         <v>845</v>
       </c>
@@ -14658,57 +14685,57 @@
       <c r="T29" s="145"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N30" s="159" t="s">
+      <c r="N30" s="164" t="s">
         <v>832</v>
       </c>
-      <c r="O30" s="160"/>
-      <c r="P30" s="160"/>
-      <c r="Q30" s="161"/>
+      <c r="O30" s="165"/>
+      <c r="P30" s="165"/>
+      <c r="Q30" s="166"/>
       <c r="R30" t="s">
         <v>851</v>
       </c>
-      <c r="S30" s="179" t="s">
+      <c r="S30" s="152" t="s">
         <v>870</v>
       </c>
-      <c r="T30" s="179"/>
+      <c r="T30" s="152"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N31" s="159" t="s">
+      <c r="N31" s="164" t="s">
         <v>833</v>
       </c>
-      <c r="O31" s="160"/>
-      <c r="P31" s="160"/>
-      <c r="Q31" s="161"/>
+      <c r="O31" s="165"/>
+      <c r="P31" s="165"/>
+      <c r="Q31" s="166"/>
       <c r="R31" t="s">
         <v>852</v>
       </c>
-      <c r="S31" s="179" t="s">
+      <c r="S31" s="152" t="s">
         <v>871</v>
       </c>
-      <c r="T31" s="179"/>
+      <c r="T31" s="152"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N32" s="159" t="s">
+      <c r="N32" s="164" t="s">
         <v>856</v>
       </c>
-      <c r="O32" s="160"/>
-      <c r="P32" s="160"/>
-      <c r="Q32" s="161"/>
+      <c r="O32" s="165"/>
+      <c r="P32" s="165"/>
+      <c r="Q32" s="166"/>
       <c r="R32" t="s">
         <v>451</v>
       </c>
-      <c r="S32" s="179" t="s">
+      <c r="S32" s="152" t="s">
         <v>872</v>
       </c>
-      <c r="T32" s="179"/>
+      <c r="T32" s="152"/>
     </row>
     <row r="33" spans="14:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N33" s="152" t="s">
+      <c r="N33" s="173" t="s">
         <v>835</v>
       </c>
-      <c r="O33" s="153"/>
-      <c r="P33" s="153"/>
-      <c r="Q33" s="154"/>
+      <c r="O33" s="174"/>
+      <c r="P33" s="174"/>
+      <c r="Q33" s="175"/>
       <c r="R33" t="s">
         <v>853</v>
       </c>
@@ -14716,19 +14743,67 @@
         <v>618</v>
       </c>
       <c r="T33" s="145"/>
-      <c r="U33" s="155"/>
-      <c r="V33" s="155"/>
-      <c r="W33" s="155"/>
-      <c r="X33" s="155"/>
+      <c r="U33" s="176"/>
+      <c r="V33" s="176"/>
+      <c r="W33" s="176"/>
+      <c r="X33" s="176"/>
     </row>
     <row r="34" spans="14:24" x14ac:dyDescent="0.25">
-      <c r="U34" s="155"/>
-      <c r="V34" s="155"/>
-      <c r="W34" s="155"/>
-      <c r="X34" s="155"/>
+      <c r="U34" s="176"/>
+      <c r="V34" s="176"/>
+      <c r="W34" s="176"/>
+      <c r="X34" s="176"/>
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U34:X34"/>
+    <mergeCell ref="R7:Y7"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="N31:Q31"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J3:Y3"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:T21"/>
     <mergeCell ref="S32:T32"/>
     <mergeCell ref="S33:T33"/>
     <mergeCell ref="D18:F18"/>
@@ -14745,54 +14820,6 @@
     <mergeCell ref="S30:T30"/>
     <mergeCell ref="S31:T31"/>
     <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J3:Y3"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="J7:Q7"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U34:X34"/>
-    <mergeCell ref="R7:Y7"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="N30:Q30"/>
-    <mergeCell ref="N31:Q31"/>
-    <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="N21:Q21"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="N26:Q26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added driving bus signal for timestamp option on RX buffer
</commit_message>
<xml_diff>
--- a/doc/core/DRV_BUS_and_more.xlsx
+++ b/doc/core/DRV_BUS_and_more.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="569">
   <si>
     <t>Index</t>
   </si>
@@ -1883,6 +1883,12 @@
   </si>
   <si>
     <t>361-365</t>
+  </si>
+  <si>
+    <t>drv_rtsopt</t>
+  </si>
+  <si>
+    <t>Receive Buffer timestamp options (Sample at the end of CAN Frame or Beginning of CAN Frame)</t>
   </si>
 </sst>
 </file>
@@ -2314,40 +2320,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2381,23 +2370,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -2701,8 +2707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3344,7 +3350,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>146</v>
+        <v>567</v>
       </c>
       <c r="D29" s="14"/>
       <c r="E29" s="14" t="s">
@@ -3353,7 +3359,9 @@
       <c r="F29" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G29" s="14"/>
+      <c r="G29" s="14" t="s">
+        <v>568</v>
+      </c>
       <c r="H29" s="8" t="s">
         <v>71</v>
       </c>
@@ -6852,33 +6860,33 @@
   <sheetData>
     <row r="2" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="49" t="s">
         <v>468</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="51" t="s">
         <v>292</v>
       </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="38"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="51"/>
+      <c r="V3" s="51"/>
+      <c r="W3" s="51"/>
+      <c r="X3" s="51"/>
+      <c r="Y3" s="52"/>
     </row>
     <row r="4" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C4" s="21"/>
@@ -6948,10 +6956,10 @@
       </c>
     </row>
     <row r="5" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="47" t="s">
         <v>466</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
@@ -7011,10 +7019,10 @@
       </c>
     </row>
     <row r="6" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="D6" s="35"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="23" t="s">
         <v>491</v>
       </c>
@@ -7080,126 +7088,126 @@
       </c>
     </row>
     <row r="7" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="38" t="s">
         <v>540</v>
       </c>
-      <c r="D7" s="46"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
-      <c r="J7" s="39" t="s">
+      <c r="J7" s="53" t="s">
         <v>519</v>
       </c>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="57" t="s">
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="55"/>
+      <c r="R7" s="32" t="s">
         <v>492</v>
       </c>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="59"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="34"/>
     </row>
     <row r="11" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="46" t="s">
         <v>456</v>
       </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
     </row>
     <row r="12" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="46" t="s">
         <v>457</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31" t="s">
+      <c r="D12" s="46"/>
+      <c r="E12" s="46" t="s">
         <v>452</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="N12" s="50" t="s">
+      <c r="F12" s="46"/>
+      <c r="N12" s="43" t="s">
         <v>492</v>
       </c>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="52"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="45"/>
       <c r="R12" s="25" t="s">
         <v>493</v>
       </c>
-      <c r="S12" s="32" t="s">
+      <c r="S12" s="56" t="s">
         <v>513</v>
       </c>
-      <c r="T12" s="33"/>
+      <c r="T12" s="57"/>
     </row>
     <row r="13" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="N13" s="47" t="s">
+      <c r="N13" s="40" t="s">
         <v>469</v>
       </c>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="49"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="42"/>
       <c r="R13" t="s">
         <v>494</v>
       </c>
-      <c r="S13" s="29" t="s">
+      <c r="S13" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T13" s="29"/>
+      <c r="T13" s="58"/>
     </row>
     <row r="14" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="N14" s="42" t="s">
+      <c r="N14" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="44"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="37"/>
       <c r="R14" t="s">
         <v>495</v>
       </c>
-      <c r="S14" s="29" t="s">
+      <c r="S14" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T14" s="29"/>
+      <c r="T14" s="58"/>
     </row>
     <row r="15" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="N15" s="42" t="s">
+      <c r="N15" s="35" t="s">
         <v>510</v>
       </c>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="44"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="37"/>
       <c r="R15" t="s">
         <v>496</v>
       </c>
-      <c r="S15" s="29" t="s">
+      <c r="S15" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T15" s="29"/>
+      <c r="T15" s="58"/>
     </row>
     <row r="16" spans="3:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N16" s="42" t="s">
+      <c r="N16" s="35" t="s">
         <v>511</v>
       </c>
-      <c r="O16" s="43"/>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="44"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="37"/>
       <c r="R16" t="s">
         <v>294</v>
       </c>
-      <c r="S16" s="29" t="s">
+      <c r="S16" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T16" s="29"/>
+      <c r="T16" s="58"/>
     </row>
     <row r="17" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="17">
@@ -7226,29 +7234,29 @@
       <c r="K17" s="19">
         <v>0</v>
       </c>
-      <c r="N17" s="42" t="s">
+      <c r="N17" s="35" t="s">
         <v>473</v>
       </c>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="44"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="37"/>
       <c r="R17" t="s">
         <v>497</v>
       </c>
-      <c r="S17" s="29" t="s">
+      <c r="S17" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T17" s="29"/>
+      <c r="T17" s="58"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>514</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
       <c r="G18" t="s">
         <v>524</v>
       </c>
@@ -7264,62 +7272,62 @@
       <c r="K18" t="s">
         <v>520</v>
       </c>
-      <c r="N18" s="42" t="s">
+      <c r="N18" s="35" t="s">
         <v>472</v>
       </c>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="44"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="37"/>
       <c r="R18" t="s">
         <v>498</v>
       </c>
-      <c r="S18" s="28" t="s">
+      <c r="S18" s="59" t="s">
         <v>514</v>
       </c>
-      <c r="T18" s="28"/>
+      <c r="T18" s="59"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>515</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
       <c r="J19" t="s">
         <v>525</v>
       </c>
       <c r="K19" t="s">
         <v>526</v>
       </c>
-      <c r="N19" s="42" t="s">
+      <c r="N19" s="35" t="s">
         <v>474</v>
       </c>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="44"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="37"/>
       <c r="R19" t="s">
         <v>499</v>
       </c>
-      <c r="S19" s="28" t="s">
+      <c r="S19" s="59" t="s">
         <v>515</v>
       </c>
-      <c r="T19" s="28"/>
+      <c r="T19" s="59"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>516</v>
       </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31" t="s">
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46" t="s">
         <v>539</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="46"/>
       <c r="H20" t="s">
         <v>530</v>
       </c>
@@ -7332,261 +7340,309 @@
       <c r="K20" t="s">
         <v>527</v>
       </c>
-      <c r="N20" s="42" t="s">
+      <c r="N20" s="35" t="s">
         <v>476</v>
       </c>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="44"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="37"/>
       <c r="R20" t="s">
         <v>296</v>
       </c>
-      <c r="S20" s="29" t="s">
+      <c r="S20" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T20" s="29"/>
+      <c r="T20" s="58"/>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>517</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
       <c r="H21" t="s">
         <v>532</v>
       </c>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="46" t="s">
         <v>531</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="N21" s="42" t="s">
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="N21" s="35" t="s">
         <v>477</v>
       </c>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="44"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="37"/>
       <c r="R21" t="s">
         <v>500</v>
       </c>
-      <c r="S21" s="29" t="s">
+      <c r="S21" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T21" s="29"/>
+      <c r="T21" s="58"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>533</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
       <c r="H22" t="s">
         <v>532</v>
       </c>
-      <c r="I22" s="31" t="s">
+      <c r="I22" s="46" t="s">
         <v>534</v>
       </c>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="N22" s="42" t="s">
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="N22" s="35" t="s">
         <v>478</v>
       </c>
-      <c r="O22" s="43"/>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="44"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="37"/>
       <c r="R22" t="s">
         <v>502</v>
       </c>
-      <c r="S22" s="29" t="s">
+      <c r="S22" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T22" s="29"/>
+      <c r="T22" s="58"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N23" s="42" t="s">
+      <c r="N23" s="35" t="s">
         <v>479</v>
       </c>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="44"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="37"/>
       <c r="R23" t="s">
         <v>503</v>
       </c>
-      <c r="S23" s="28" t="s">
+      <c r="S23" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="T23" s="28"/>
+      <c r="T23" s="59"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N24" s="42" t="s">
+      <c r="N24" s="35" t="s">
         <v>480</v>
       </c>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="44"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="37"/>
       <c r="R24" t="s">
         <v>297</v>
       </c>
-      <c r="S24" s="29" t="s">
+      <c r="S24" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T24" s="29"/>
+      <c r="T24" s="58"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N25" s="42" t="s">
+      <c r="N25" s="35" t="s">
         <v>481</v>
       </c>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="44"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="37"/>
       <c r="R25" t="s">
         <v>504</v>
       </c>
-      <c r="S25" s="29" t="s">
+      <c r="S25" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T25" s="29"/>
+      <c r="T25" s="58"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N26" s="42" t="s">
+      <c r="N26" s="35" t="s">
         <v>482</v>
       </c>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="44"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="37"/>
       <c r="R26" t="s">
         <v>505</v>
       </c>
-      <c r="S26" s="29" t="s">
+      <c r="S26" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T26" s="29"/>
+      <c r="T26" s="58"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N27" s="42" t="s">
+      <c r="N27" s="35" t="s">
         <v>483</v>
       </c>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="44"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="37"/>
       <c r="R27" t="s">
         <v>506</v>
       </c>
-      <c r="S27" s="29" t="s">
+      <c r="S27" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T27" s="29"/>
+      <c r="T27" s="58"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N28" s="42" t="s">
+      <c r="N28" s="35" t="s">
         <v>486</v>
       </c>
-      <c r="O28" s="43"/>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="44"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="37"/>
       <c r="R28" t="s">
         <v>298</v>
       </c>
-      <c r="S28" s="29" t="s">
+      <c r="S28" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T28" s="29"/>
+      <c r="T28" s="58"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N29" s="42" t="s">
+      <c r="N29" s="35" t="s">
         <v>487</v>
       </c>
-      <c r="O29" s="43"/>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="44"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="37"/>
       <c r="R29" t="s">
         <v>501</v>
       </c>
-      <c r="S29" s="29" t="s">
+      <c r="S29" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T29" s="29"/>
+      <c r="T29" s="58"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N30" s="42" t="s">
+      <c r="N30" s="35" t="s">
         <v>488</v>
       </c>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="44"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="37"/>
       <c r="R30" t="s">
         <v>507</v>
       </c>
-      <c r="S30" s="28" t="s">
+      <c r="S30" s="59" t="s">
         <v>516</v>
       </c>
-      <c r="T30" s="28"/>
+      <c r="T30" s="59"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N31" s="42" t="s">
+      <c r="N31" s="35" t="s">
         <v>489</v>
       </c>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="44"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="37"/>
       <c r="R31" t="s">
         <v>508</v>
       </c>
-      <c r="S31" s="28" t="s">
+      <c r="S31" s="59" t="s">
         <v>517</v>
       </c>
-      <c r="T31" s="28"/>
+      <c r="T31" s="59"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="N32" s="42" t="s">
+      <c r="N32" s="35" t="s">
         <v>512</v>
       </c>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="44"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="37"/>
       <c r="R32" t="s">
         <v>299</v>
       </c>
-      <c r="S32" s="28" t="s">
+      <c r="S32" s="59" t="s">
         <v>518</v>
       </c>
-      <c r="T32" s="28"/>
+      <c r="T32" s="59"/>
     </row>
     <row r="33" spans="14:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N33" s="53" t="s">
+      <c r="N33" s="28" t="s">
         <v>491</v>
       </c>
-      <c r="O33" s="54"/>
-      <c r="P33" s="54"/>
-      <c r="Q33" s="55"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="30"/>
       <c r="R33" t="s">
         <v>509</v>
       </c>
-      <c r="S33" s="29" t="s">
+      <c r="S33" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="T33" s="29"/>
-      <c r="U33" s="56"/>
-      <c r="V33" s="56"/>
-      <c r="W33" s="56"/>
-      <c r="X33" s="56"/>
+      <c r="T33" s="58"/>
+      <c r="U33" s="31"/>
+      <c r="V33" s="31"/>
+      <c r="W33" s="31"/>
+      <c r="X33" s="31"/>
     </row>
     <row r="34" spans="14:24" x14ac:dyDescent="0.25">
-      <c r="U34" s="56"/>
-      <c r="V34" s="56"/>
-      <c r="W34" s="56"/>
-      <c r="X34" s="56"/>
+      <c r="U34" s="31"/>
+      <c r="V34" s="31"/>
+      <c r="W34" s="31"/>
+      <c r="X34" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J3:Y3"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
     <mergeCell ref="N33:Q33"/>
     <mergeCell ref="U33:X33"/>
     <mergeCell ref="U34:X34"/>
@@ -7603,54 +7659,6 @@
     <mergeCell ref="N24:Q24"/>
     <mergeCell ref="N25:Q25"/>
     <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J3:Y3"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="J7:Q7"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="S22:T22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>